<commit_message>
change cost field to numbe
for change cost field to number; country name mapping; and increase the session timeout
</commit_message>
<xml_diff>
--- a/Freight/TemplateFile/DHL_Ratecard_Template_09022021.xlsx
+++ b/Freight/TemplateFile/DHL_Ratecard_Template_09022021.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="7170" windowWidth="28830" windowHeight="7230" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="7170" windowWidth="28830" windowHeight="7230" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Export_WW_Doc_up_to_2Kg" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4004" uniqueCount="2320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4004" uniqueCount="2319">
   <si>
     <t>0.5</t>
   </si>
@@ -6969,37 +6969,34 @@
     <t>Destination zone</t>
   </si>
   <si>
-    <t>Shenzhen (SZX)</t>
-  </si>
-  <si>
-    <t>Fuzhou (FOC)</t>
-  </si>
-  <si>
-    <t>South China Area (HAK)</t>
-  </si>
-  <si>
-    <t>Chaoshan &amp; Huizhou (SWA)</t>
-  </si>
-  <si>
-    <t>Zhujiang Delta Area (ZUH)</t>
-  </si>
-  <si>
-    <t>Guangzhou (CAN)</t>
-  </si>
-  <si>
-    <t>Dongguan (DGM)</t>
-  </si>
-  <si>
-    <t>Fujian Province (XMN)</t>
-  </si>
-  <si>
-    <t>Rest of China (CN)</t>
-  </si>
-  <si>
-    <t>Dongguan (DGM</t>
-  </si>
-  <si>
     <t>Country/Territory</t>
+  </si>
+  <si>
+    <t>China Shenzhen (SZX)</t>
+  </si>
+  <si>
+    <t>China Fuzhou (FOC)</t>
+  </si>
+  <si>
+    <t>China South China Area (HAK)</t>
+  </si>
+  <si>
+    <t>China Chaoshan &amp; Huizhou (SWA)</t>
+  </si>
+  <si>
+    <t>China Zhujiang Delta Area (ZUH)</t>
+  </si>
+  <si>
+    <t>China Guangzhou (CAN)</t>
+  </si>
+  <si>
+    <t>China Dongguan (DGM</t>
+  </si>
+  <si>
+    <t>China Fujian Province (XMN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China Rest of China (CN)  </t>
   </si>
 </sst>
 </file>
@@ -7052,7 +7049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -7067,6 +7064,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7373,7 +7371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9897,7 +9895,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="4" t="s">
-        <v>2319</v>
+        <v>2309</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1488</v>
@@ -14638,7 +14636,7 @@
   <dimension ref="A1:M242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:B242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14651,7 +14649,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="4" t="s">
-        <v>2319</v>
+        <v>2309</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1488</v>
@@ -14995,7 +14993,7 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>2309</v>
+        <v>2310</v>
       </c>
       <c r="B44" t="s">
         <v>1516</v>
@@ -15013,7 +15011,7 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
-        <v>2310</v>
+        <v>2311</v>
       </c>
       <c r="B45" t="s">
         <v>1516</v>
@@ -15031,7 +15029,7 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="s">
-        <v>2311</v>
+        <v>2312</v>
       </c>
       <c r="B46" t="s">
         <v>1516</v>
@@ -15048,8 +15046,8 @@
       <c r="M46" s="3"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" t="s">
-        <v>2312</v>
+      <c r="A47" s="6" t="s">
+        <v>2313</v>
       </c>
       <c r="B47" t="s">
         <v>1516</v>
@@ -15066,8 +15064,8 @@
       <c r="M47" s="3"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" t="s">
-        <v>2313</v>
+      <c r="A48" s="6" t="s">
+        <v>2314</v>
       </c>
       <c r="B48" t="s">
         <v>1516</v>
@@ -15084,8 +15082,8 @@
       <c r="M48" s="3"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" t="s">
-        <v>2314</v>
+      <c r="A49" s="6" t="s">
+        <v>2315</v>
       </c>
       <c r="B49" t="s">
         <v>1516</v>
@@ -15102,8 +15100,8 @@
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" t="s">
-        <v>2318</v>
+      <c r="A50" s="6" t="s">
+        <v>2316</v>
       </c>
       <c r="B50" t="s">
         <v>1516</v>
@@ -15120,8 +15118,8 @@
       <c r="M50" s="3"/>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" t="s">
-        <v>2316</v>
+      <c r="A51" s="6" t="s">
+        <v>2317</v>
       </c>
       <c r="B51" t="s">
         <v>1516</v>
@@ -15138,8 +15136,8 @@
       <c r="M51" s="3"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" t="s">
-        <v>2317</v>
+      <c r="A52" s="6" t="s">
+        <v>2318</v>
       </c>
       <c r="B52" t="s">
         <v>1540</v>
@@ -15156,7 +15154,7 @@
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" t="s">
+      <c r="A53" s="6" t="s">
         <v>1676</v>
       </c>
       <c r="B53" t="s">
@@ -20029,7 +20027,7 @@
   <dimension ref="A1:N242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20040,7 +20038,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="4" t="s">
-        <v>2319</v>
+        <v>2309</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1488</v>
@@ -20384,7 +20382,7 @@
     </row>
     <row r="44" spans="1:14" ht="14.45" customHeight="1">
       <c r="A44" t="s">
-        <v>2309</v>
+        <v>2310</v>
       </c>
       <c r="B44" t="s">
         <v>1516</v>
@@ -20402,7 +20400,7 @@
     </row>
     <row r="45" spans="1:14" ht="14.45" customHeight="1">
       <c r="A45" t="s">
-        <v>2310</v>
+        <v>2311</v>
       </c>
       <c r="B45" t="s">
         <v>1516</v>
@@ -20420,7 +20418,7 @@
     </row>
     <row r="46" spans="1:14" ht="14.45" customHeight="1">
       <c r="A46" t="s">
-        <v>2311</v>
+        <v>2312</v>
       </c>
       <c r="B46" t="s">
         <v>1516</v>
@@ -20438,7 +20436,7 @@
     </row>
     <row r="47" spans="1:14" ht="14.45" customHeight="1">
       <c r="A47" t="s">
-        <v>2312</v>
+        <v>2313</v>
       </c>
       <c r="B47" t="s">
         <v>1516</v>
@@ -20456,7 +20454,7 @@
     </row>
     <row r="48" spans="1:14" ht="14.45" customHeight="1">
       <c r="A48" t="s">
-        <v>2313</v>
+        <v>2314</v>
       </c>
       <c r="B48" t="s">
         <v>1516</v>
@@ -20474,7 +20472,7 @@
     </row>
     <row r="49" spans="1:14" ht="14.45" customHeight="1">
       <c r="A49" t="s">
-        <v>2314</v>
+        <v>2315</v>
       </c>
       <c r="B49" t="s">
         <v>1516</v>
@@ -20492,7 +20490,7 @@
     </row>
     <row r="50" spans="1:14" ht="14.45" customHeight="1">
       <c r="A50" t="s">
-        <v>2315</v>
+        <v>2316</v>
       </c>
       <c r="B50" t="s">
         <v>1516</v>
@@ -20510,7 +20508,7 @@
     </row>
     <row r="51" spans="1:14" ht="14.45" customHeight="1">
       <c r="A51" t="s">
-        <v>2316</v>
+        <v>2317</v>
       </c>
       <c r="B51" t="s">
         <v>1516</v>
@@ -20528,7 +20526,7 @@
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>2317</v>
+        <v>2318</v>
       </c>
       <c r="B52" t="s">
         <v>1672</v>
@@ -22264,15 +22262,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010049382FB7CD94B94393E79ED27ABC7761" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c9ee4f9c00eb65f4095902d87160552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7d3fa97a-df71-4cba-8947-dc1770271724" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6e6f73c273967a2085d941db8e08e76a" ns2:_="">
     <xsd:import namespace="7d3fa97a-df71-4cba-8947-dc1770271724"/>
@@ -22430,6 +22419,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -22437,14 +22435,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{621AB76E-FF18-496F-A035-22106405C7BA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3522D8FC-B204-42D5-AFD4-8948C0502AAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22462,6 +22452,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{621AB76E-FF18-496F-A035-22106405C7BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A131E1DC-8102-4FF2-954B-36C4553E7F68}">
   <ds:schemaRefs>

</xml_diff>